<commit_message>
Updated Gantt Chart. Created webpage, client & server side javascript, USNO API Call module. We probably have to manually put in the rest of the data.
</commit_message>
<xml_diff>
--- a/Documents/Gantt Chart.xlsx
+++ b/Documents/Gantt Chart.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="30">
   <si>
     <t>Setup User Interface of Nightsky Webpage</t>
   </si>
@@ -105,13 +105,22 @@
   </si>
   <si>
     <t>Jerry</t>
+  </si>
+  <si>
+    <t>CANCELLED</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          Get node.js server to communicate with USNO API</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Progress Bar: </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -121,6 +130,14 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <strike/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -157,7 +174,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -171,11 +188,60 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="9">
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -244,50 +310,6 @@
         <scheme val="minor"/>
       </font>
     </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -301,14 +323,289 @@
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>406400</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="Rectangle 2"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4305300" y="2032000"/>
+          <a:ext cx="2362200" cy="209550"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>12700</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1047750</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="Rectangle 3"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4318000" y="2965450"/>
+          <a:ext cx="2990850" cy="190500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>6350</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1479550</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="Rectangle 4"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4311650" y="3898900"/>
+          <a:ext cx="1473200" cy="184150"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>6350</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>12700</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="Rectangle 5"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4311650" y="4641850"/>
+          <a:ext cx="1962150" cy="165100"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>12700</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>2241550</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="Rectangle 6"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4318000" y="939800"/>
+          <a:ext cx="4184650" cy="165100"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A2:E24" headerRowCount="0" totalsRowShown="0" headerRowDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A2:E26" headerRowCount="0" totalsRowShown="0" headerRowDxfId="8">
   <tableColumns count="5">
-    <tableColumn id="1" name="Column1" headerRowDxfId="0"/>
-    <tableColumn id="2" name="Column2" headerRowDxfId="1"/>
-    <tableColumn id="3" name="Column3" headerRowDxfId="2" dataDxfId="8"/>
-    <tableColumn id="4" name="Column4" headerRowDxfId="3" dataDxfId="7"/>
-    <tableColumn id="5" name="Column5" headerRowDxfId="4" dataDxfId="6"/>
+    <tableColumn id="1" name="Column1" headerRowDxfId="7"/>
+    <tableColumn id="2" name="Column2" headerRowDxfId="6"/>
+    <tableColumn id="3" name="Column3" headerRowDxfId="5" dataDxfId="4"/>
+    <tableColumn id="4" name="Column4" headerRowDxfId="3" dataDxfId="2"/>
+    <tableColumn id="5" name="Column5" headerRowDxfId="1" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
@@ -577,10 +874,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E24"/>
+  <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -635,7 +932,7 @@
         <v>42799</v>
       </c>
       <c r="E4" s="6">
-        <v>0</v>
+        <v>90</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
@@ -652,10 +949,13 @@
         <v>42799</v>
       </c>
       <c r="E5" s="6">
-        <v>0</v>
+        <v>90</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6" s="8" t="s">
+        <v>29</v>
+      </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
       <c r="E6" s="6"/>
@@ -681,11 +981,11 @@
         <v>42806</v>
       </c>
       <c r="E8" s="6">
-        <v>0</v>
+        <v>75</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
+      <c r="A9" s="7" t="s">
         <v>18</v>
       </c>
       <c r="B9" t="s">
@@ -697,16 +997,16 @@
       <c r="D9" s="3">
         <v>42813</v>
       </c>
-      <c r="E9" s="6">
-        <v>0</v>
+      <c r="E9" s="6" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>20</v>
+      <c r="A10" s="9" t="s">
+        <v>28</v>
       </c>
       <c r="B10" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C10" s="3">
         <v>42807</v>
@@ -717,36 +1017,39 @@
       <c r="E10" s="6"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="6"/>
-    </row>
-    <row r="12" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A12" s="2" t="s">
+      <c r="A11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" s="3">
+        <v>42807</v>
+      </c>
+      <c r="D11" s="3">
+        <v>42813</v>
+      </c>
+      <c r="E11" s="6">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="6"/>
+    </row>
+    <row r="13" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A13" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E12" s="6"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>11</v>
-      </c>
-      <c r="B13" t="s">
-        <v>26</v>
-      </c>
-      <c r="C13" s="3">
-        <v>42800</v>
-      </c>
-      <c r="D13" s="3">
-        <v>42806</v>
-      </c>
-      <c r="E13" s="6">
-        <v>0</v>
-      </c>
+      <c r="E13" s="6"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B14" t="s">
         <v>26</v>
@@ -758,57 +1061,60 @@
         <v>42806</v>
       </c>
       <c r="E14" s="6">
-        <v>0</v>
+        <v>60</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B15" t="s">
         <v>26</v>
       </c>
       <c r="C15" s="3">
+        <v>42800</v>
+      </c>
+      <c r="D15" s="3">
+        <v>42806</v>
+      </c>
+      <c r="E15" s="6">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16" t="s">
+        <v>26</v>
+      </c>
+      <c r="C16" s="3">
         <v>42807</v>
       </c>
-      <c r="D15" s="3">
+      <c r="D16" s="3">
         <v>42813</v>
       </c>
-      <c r="E15" s="6">
+      <c r="E16" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="6"/>
-    </row>
-    <row r="17" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="2" t="s">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>29</v>
+      </c>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="6"/>
+    </row>
+    <row r="18" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A18" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E17" s="6"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
-        <v>16</v>
-      </c>
-      <c r="B18" t="s">
-        <v>25</v>
-      </c>
-      <c r="C18" s="3">
-        <v>42807</v>
-      </c>
-      <c r="D18" s="3">
-        <v>42813</v>
-      </c>
-      <c r="E18" s="6">
-        <v>0</v>
-      </c>
+      <c r="E18" s="6"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B19" t="s">
         <v>25</v>
@@ -820,15 +1126,15 @@
         <v>42813</v>
       </c>
       <c r="E19" s="6">
-        <v>0</v>
+        <v>40</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B20" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C20" s="3">
         <v>42807</v>
@@ -841,53 +1147,82 @@
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="E21" s="6"/>
-    </row>
-    <row r="22" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A22" s="2" t="s">
+      <c r="A21" t="s">
+        <v>17</v>
+      </c>
+      <c r="B21" t="s">
+        <v>26</v>
+      </c>
+      <c r="C21" s="3">
+        <v>42807</v>
+      </c>
+      <c r="D21" s="3">
+        <v>42813</v>
+      </c>
+      <c r="E21" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>29</v>
+      </c>
+      <c r="E22" s="6"/>
+    </row>
+    <row r="23" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A23" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E22" s="6"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A23" t="s">
-        <v>22</v>
-      </c>
-      <c r="B23" t="s">
-        <v>23</v>
-      </c>
-      <c r="C23" s="3">
-        <v>42800</v>
-      </c>
-      <c r="D23" s="3">
-        <v>42803</v>
-      </c>
-      <c r="E23" s="6">
-        <v>0</v>
-      </c>
+      <c r="E23" s="6"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B24" t="s">
         <v>23</v>
       </c>
       <c r="C24" s="3">
+        <v>42800</v>
+      </c>
+      <c r="D24" s="3">
+        <v>42803</v>
+      </c>
+      <c r="E24" s="6">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
+        <v>23</v>
+      </c>
+      <c r="C25" s="3">
         <v>42807</v>
       </c>
-      <c r="D24" s="3">
+      <c r="D25" s="3">
         <v>42814</v>
       </c>
-      <c r="E24" s="6">
+      <c r="E25" s="6">
         <v>0</v>
       </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>29</v>
+      </c>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>